<commit_message>
[fix] - fix AC datatable and dashboard query
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/AC_Coming.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/AC_Coming.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>STT</t>
   </si>
@@ -61,48 +61,6 @@
   </si>
   <si>
     <t>Quốc gia</t>
-  </si>
-  <si>
-    <t>Timofey Epanchintsev</t>
-  </si>
-  <si>
-    <t>timepanc@ural.edu.com</t>
-  </si>
-  <si>
-    <t>Ural Federal University</t>
-  </si>
-  <si>
-    <t>Russian Federation (the)</t>
-  </si>
-  <si>
-    <t>11-03-2019</t>
-  </si>
-  <si>
-    <t>13-03-2019</t>
-  </si>
-  <si>
-    <t>Đã hoàn thành</t>
-  </si>
-  <si>
-    <t>Có hỗ trợ</t>
-  </si>
-  <si>
-    <t>Maisarah Ahmad</t>
-  </si>
-  <si>
-    <t>maiah@utp.edu.com</t>
-  </si>
-  <si>
-    <t>Universiti Teknologi Petronas</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>08-07-2019</t>
-  </si>
-  <si>
-    <t>19-07-2019</t>
   </si>
 </sst>
 </file>
@@ -478,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3BF669-474F-40E8-A464-8D626F6933B9}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -548,66 +506,6 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="4"/>
-    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="H1:H2"/>

</xml_diff>

<commit_message>
[fix] - fix AC datatable and dashboard query (#1261)
Co-authored-by: Quoc Tuan <39939107+quoctuanck99@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/AC_Coming.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/AC_Coming.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>STT</t>
   </si>
@@ -61,48 +61,6 @@
   </si>
   <si>
     <t>Quốc gia</t>
-  </si>
-  <si>
-    <t>Timofey Epanchintsev</t>
-  </si>
-  <si>
-    <t>timepanc@ural.edu.com</t>
-  </si>
-  <si>
-    <t>Ural Federal University</t>
-  </si>
-  <si>
-    <t>Russian Federation (the)</t>
-  </si>
-  <si>
-    <t>11-03-2019</t>
-  </si>
-  <si>
-    <t>13-03-2019</t>
-  </si>
-  <si>
-    <t>Đã hoàn thành</t>
-  </si>
-  <si>
-    <t>Có hỗ trợ</t>
-  </si>
-  <si>
-    <t>Maisarah Ahmad</t>
-  </si>
-  <si>
-    <t>maiah@utp.edu.com</t>
-  </si>
-  <si>
-    <t>Universiti Teknologi Petronas</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>08-07-2019</t>
-  </si>
-  <si>
-    <t>19-07-2019</t>
   </si>
 </sst>
 </file>
@@ -478,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3BF669-474F-40E8-A464-8D626F6933B9}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -548,66 +506,6 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="4"/>
-    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="H1:H2"/>

</xml_diff>